<commit_message>
assign 4 working commit
</commit_message>
<xml_diff>
--- a/Assignment_3/images/pai.xlsx
+++ b/Assignment_3/images/pai.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/michaelrocchio/git/msds_410/Assignment_3/images/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{51CD7A4F-F887-734B-B567-759780C3838B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DAD7A4-E8B9-0B4A-9769-A777E4FE5B31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="860" windowWidth="41120" windowHeight="25720" xr2:uid="{6A5A49DF-EB8B-594B-A639-3A1AAA13BCDB}"/>
   </bookViews>
@@ -444,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0702A71B-741C-B84C-A2DC-B6375A4D7BB8}">
-  <dimension ref="B1:G14"/>
+  <dimension ref="B1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -455,7 +455,7 @@
     <col min="2" max="3" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>16</v>
       </c>
@@ -464,7 +464,7 @@
         <v>7254.74</v>
       </c>
     </row>
-    <row r="2" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>15</v>
       </c>
@@ -474,14 +474,14 @@
       <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -491,25 +491,36 @@
       <c r="E3">
         <v>425.55</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3">
+        <f>D3-E3</f>
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>1</v>
       </c>
       <c r="D4">
         <v>1480.98</v>
       </c>
+      <c r="E4">
+        <v>180.98</v>
+      </c>
       <c r="F4">
+        <f t="shared" ref="F4:F11" si="0">D4-E4</f>
+        <v>1300</v>
+      </c>
+      <c r="G4">
         <v>26.99</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>2</v>
       </c>
@@ -517,10 +528,14 @@
         <v>4780.3500000000004</v>
       </c>
       <c r="F5">
+        <f t="shared" si="0"/>
+        <v>4780.3500000000004</v>
+      </c>
+      <c r="G5">
         <v>27.99</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>10</v>
       </c>
@@ -528,21 +543,32 @@
         <v>1357.36</v>
       </c>
       <c r="F6">
+        <f t="shared" si="0"/>
+        <v>1357.36</v>
+      </c>
+      <c r="G6">
         <v>28.74</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>9</v>
       </c>
       <c r="D7">
         <v>1208.17</v>
       </c>
+      <c r="E7">
+        <v>208.17</v>
+      </c>
       <c r="F7">
+        <f t="shared" si="0"/>
+        <v>1000.0000000000001</v>
+      </c>
+      <c r="G7">
         <v>29.99</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>11</v>
       </c>
@@ -553,13 +579,17 @@
         <v>428.03</v>
       </c>
       <c r="F8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G8">
         <v>31.99</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>13</v>
       </c>
@@ -570,13 +600,17 @@
         <v>507.49</v>
       </c>
       <c r="F9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9">
         <v>30.24</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>14</v>
       </c>
@@ -587,39 +621,61 @@
         <v>1972.76</v>
       </c>
       <c r="E10">
-        <v>1950</v>
+        <f>1950+C10</f>
+        <v>2004.57</v>
       </c>
       <c r="F10">
+        <f t="shared" si="0"/>
+        <v>-31.809999999999945</v>
+      </c>
+      <c r="G10">
         <v>21.9</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>17</v>
       </c>
       <c r="D11">
         <v>8992.16</v>
       </c>
+      <c r="E11">
+        <v>1068.9000000000001</v>
+      </c>
       <c r="F11">
+        <f t="shared" si="0"/>
+        <v>7923.26</v>
+      </c>
+      <c r="G11">
         <v>28.99</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <f>SUM(D3:D11)</f>
+        <v>21152.85</v>
+      </c>
+      <c r="F12">
+        <f t="shared" ref="E12:F12" si="1">SUM(F3:F11)</f>
+        <v>16329.160000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D13" t="s">
         <v>4</v>
       </c>
       <c r="E13">
         <f>SUM(E3:E11)</f>
-        <v>3311.0699999999997</v>
-      </c>
-    </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+        <v>4823.6900000000005</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="D14" t="s">
         <v>18</v>
       </c>
       <c r="E14">
         <f>C1-E13</f>
-        <v>3943.67</v>
+        <v>2431.0499999999993</v>
       </c>
     </row>
   </sheetData>

</xml_diff>